<commit_message>
fix chart labels and formatting
</commit_message>
<xml_diff>
--- a/paper/final/Top 50 vulnerabilities by year - cvedetails.xlsx
+++ b/paper/final/Top 50 vulnerabilities by year - cvedetails.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\furry\Git\NYU-CS-GY-6813\paper\papers\final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\furry\Git\NYU-CS-GY-6813\paper\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980DAF20-BC80-44EC-B2E7-C434CF777550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D81FD7-5454-4DDC-A6D5-31F4CE880723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5176,6 +5176,40 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Vulnerabilities (Log10)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5995,12 +6029,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr lang="en-US" sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -6043,7 +6074,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="75000"/>
@@ -6099,7 +6130,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="75000"/>
@@ -6153,12 +6184,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -6354,12 +6382,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -6399,6 +6424,28 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Vulnerabilities (Log10)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6412,12 +6459,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -6444,12 +6488,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -6486,12 +6527,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr rtl="0">
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -6541,7 +6579,14 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1400"/>
+        <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -6752,7 +6797,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -6996,6 +7043,37 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Vulnerabilities (Log10)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -28120,8 +28198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>